<commit_message>
antes de testar retirar apenas os 10 pixeis centrais para a sampple
</commit_message>
<xml_diff>
--- a/Intervalos HSV resistências.xlsx
+++ b/Intervalos HSV resistências.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajmr1\Documents\VCWORK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E14658-2158-4F0B-9583-AC4FC835B185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530394D3-8164-4E88-AEB7-5D8BF39C8EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F9ACC887-9164-4597-A4CE-241EF22D55D3}"/>
+    <workbookView xWindow="195" yWindow="1710" windowWidth="28800" windowHeight="15345" xr2:uid="{F9ACC887-9164-4597-A4CE-241EF22D55D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -236,7 +236,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -334,7 +334,6 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -347,7 +346,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -700,7 +699,7 @@
   <dimension ref="A1:W58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,22 +755,22 @@
       <c r="L1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="42" t="s">
+      <c r="R1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="43" t="s">
+      <c r="S1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="42" t="s">
+      <c r="T1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="43" t="s">
+      <c r="U1" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="V1" s="44" t="s">
+      <c r="V1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="W1" s="45" t="s">
+      <c r="W1" s="44" t="s">
         <v>8</v>
       </c>
     </row>
@@ -816,10 +815,10 @@
         <f t="shared" ref="L2:L57" si="2">H2*255</f>
         <v>216.75</v>
       </c>
-      <c r="Q2" s="46" t="s">
+      <c r="Q2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="39">
+      <c r="R2" s="38">
         <f t="shared" ref="R2:R8" si="3">_xlfn.MINIFS(C:C,$B:$B,$Q2)</f>
         <v>220</v>
       </c>
@@ -827,7 +826,7 @@
         <f>_xlfn.MAXIFS(D:D,$B:$B,$Q2)</f>
         <v>251</v>
       </c>
-      <c r="T2" s="39">
+      <c r="T2" s="38">
         <f t="shared" ref="T2:T8" si="4">_xlfn.MINIFS(I:I,$B:$B,$Q2)</f>
         <v>0</v>
       </c>
@@ -885,30 +884,30 @@
         <f t="shared" si="2"/>
         <v>114.75</v>
       </c>
-      <c r="Q3" s="47" t="s">
+      <c r="Q3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="40">
+      <c r="R3" s="39">
         <f t="shared" si="3"/>
         <v>174</v>
       </c>
-      <c r="S3" s="36">
+      <c r="S3" s="35">
         <f t="shared" ref="S3:S8" si="7">_xlfn.MAXIFS(D:D,$B:$B,$Q3)</f>
         <v>185</v>
       </c>
-      <c r="T3" s="40">
+      <c r="T3" s="39">
         <f t="shared" si="4"/>
         <v>76.5</v>
       </c>
-      <c r="U3" s="36">
+      <c r="U3" s="35">
         <f t="shared" ref="U3:W8" si="8">_xlfn.MAXIFS(J:J,$B:$B,$Q3)</f>
         <v>119.85</v>
       </c>
-      <c r="V3" s="35">
+      <c r="V3" s="12">
         <f t="shared" si="5"/>
         <v>102</v>
       </c>
-      <c r="W3" s="36">
+      <c r="W3" s="35">
         <f t="shared" si="8"/>
         <v>114.75</v>
       </c>
@@ -954,30 +953,30 @@
         <f t="shared" si="2"/>
         <v>145.35</v>
       </c>
-      <c r="Q4" s="47" t="s">
+      <c r="Q4" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="R4" s="40">
+      <c r="R4" s="39">
         <f t="shared" si="3"/>
         <v>318</v>
       </c>
-      <c r="S4" s="36">
+      <c r="S4" s="35">
         <f t="shared" si="7"/>
         <v>360</v>
       </c>
-      <c r="T4" s="40">
+      <c r="T4" s="39">
         <f t="shared" si="4"/>
         <v>73.949999999999989</v>
       </c>
-      <c r="U4" s="36">
+      <c r="U4" s="35">
         <f t="shared" si="8"/>
         <v>142.80000000000001</v>
       </c>
-      <c r="V4" s="35">
+      <c r="V4" s="12">
         <f t="shared" si="5"/>
         <v>135.15</v>
       </c>
-      <c r="W4" s="36">
+      <c r="W4" s="35">
         <f t="shared" si="8"/>
         <v>145.35</v>
       </c>
@@ -1023,30 +1022,30 @@
         <f t="shared" si="2"/>
         <v>183.6</v>
       </c>
-      <c r="Q5" s="47" t="s">
+      <c r="Q5" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="R5" s="40">
+      <c r="R5" s="39">
         <f t="shared" si="3"/>
         <v>177</v>
       </c>
-      <c r="S5" s="36">
+      <c r="S5" s="35">
         <f t="shared" si="7"/>
         <v>195</v>
       </c>
-      <c r="T5" s="40">
+      <c r="T5" s="39">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U5" s="36">
+      <c r="U5" s="35">
         <f t="shared" si="8"/>
         <v>255</v>
       </c>
-      <c r="V5" s="35">
+      <c r="V5" s="12">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W5" s="36">
+      <c r="W5" s="35">
         <f t="shared" si="8"/>
         <v>198.9</v>
       </c>
@@ -1092,32 +1091,32 @@
         <f t="shared" ref="L6:L39" si="12">H6*255</f>
         <v>214.2</v>
       </c>
-      <c r="Q6" s="47" t="s">
+      <c r="Q6" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="R6" s="40">
+      <c r="R6" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S6" s="36">
+        <v>170</v>
+      </c>
+      <c r="S6" s="35">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T6" s="40">
+        <v>199</v>
+      </c>
+      <c r="T6" s="39">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U6" s="36">
+      <c r="U6" s="35">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V6" s="35">
+        <v>235.875</v>
+      </c>
+      <c r="V6" s="12">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W6" s="36">
+      <c r="W6" s="35">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>104.55</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -1161,30 +1160,30 @@
         <f t="shared" si="12"/>
         <v>193.8</v>
       </c>
-      <c r="Q7" s="47" t="s">
+      <c r="Q7" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="40">
+      <c r="R7" s="39">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S7" s="36">
+      <c r="S7" s="35">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="T7" s="40">
+      <c r="T7" s="39">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U7" s="36">
+      <c r="U7" s="35">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="V7" s="35">
+      <c r="V7" s="12">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W7" s="36">
+      <c r="W7" s="35">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -1230,30 +1229,30 @@
         <f t="shared" si="12"/>
         <v>198.9</v>
       </c>
-      <c r="Q8" s="48" t="s">
+      <c r="Q8" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="R8" s="41">
+      <c r="R8" s="40">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S8" s="38">
+      <c r="S8" s="37">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="T8" s="41">
+      <c r="T8" s="40">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U8" s="38">
+      <c r="U8" s="37">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="V8" s="37">
+      <c r="V8" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W8" s="38">
+      <c r="W8" s="37">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -1265,27 +1264,39 @@
       <c r="B9" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
+      <c r="C9" s="13">
+        <v>170</v>
+      </c>
+      <c r="D9" s="14">
+        <v>199</v>
+      </c>
+      <c r="E9" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="F9" s="22">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="G9" s="21">
+        <v>0.34</v>
+      </c>
+      <c r="H9" s="22">
+        <v>0.41</v>
+      </c>
       <c r="I9" s="23">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>204</v>
       </c>
       <c r="J9" s="24">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>235.875</v>
       </c>
       <c r="K9" s="23">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>86.7</v>
       </c>
       <c r="L9" s="24">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>104.55</v>
       </c>
       <c r="R9" s="12"/>
       <c r="S9" s="12"/>

</xml_diff>